<commit_message>
Trabalhando com Planilhas do Excel
</commit_message>
<xml_diff>
--- a/Exercicios/Análise de dados/Cusro_Python_Pandas_Digital_Innovation-master/datasets/Recife.xlsx
+++ b/Exercicios/Análise de dados/Cusro_Python_Pandas_Digital_Innovation-master/datasets/Recife.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftspu\OneDrive\Documentos\Material Curso\Painel2.1_Vendas\Dados\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rodri\OneDrive\Python\Exercicios\Análise de dados\Cusro_Python_Pandas_Digital_Innovation-master\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06A6B8EB-2696-4EEC-83D7-34816D7FEA91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="6">
   <si>
     <t>Cidade</t>
   </si>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;R$&quot;#,##0.00"/>
   </numFmts>
@@ -109,14 +110,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:E143" totalsRowShown="0">
-  <autoFilter ref="A1:E143"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:E150" totalsRowShown="0">
+  <autoFilter ref="A1:E150" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Cidade"/>
-    <tableColumn id="2" name="Data" dataDxfId="1"/>
-    <tableColumn id="3" name="Vendas" dataDxfId="0"/>
-    <tableColumn id="4" name="LojaID"/>
-    <tableColumn id="5" name="Qtde"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Cidade"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Data" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Vendas" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="LojaID"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Qtde"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -384,11 +385,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E143"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E150"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
+      <selection activeCell="B149" sqref="B149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2831,6 +2832,104 @@
         <v>8</v>
       </c>
     </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>5</v>
+      </c>
+      <c r="B144" s="1">
+        <v>43526</v>
+      </c>
+      <c r="D144">
+        <v>983</v>
+      </c>
+      <c r="E144">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>5</v>
+      </c>
+      <c r="B145" s="1">
+        <v>43527</v>
+      </c>
+      <c r="D145">
+        <v>983</v>
+      </c>
+      <c r="E145">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>5</v>
+      </c>
+      <c r="B146" s="1">
+        <v>43528</v>
+      </c>
+      <c r="D146">
+        <v>983</v>
+      </c>
+      <c r="E146">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>5</v>
+      </c>
+      <c r="B147" s="1">
+        <v>43529</v>
+      </c>
+      <c r="D147">
+        <v>983</v>
+      </c>
+      <c r="E147">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>5</v>
+      </c>
+      <c r="B148" s="1">
+        <v>43530</v>
+      </c>
+      <c r="D148">
+        <v>983</v>
+      </c>
+      <c r="E148">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>5</v>
+      </c>
+      <c r="B149" s="1">
+        <v>43531</v>
+      </c>
+      <c r="D149">
+        <v>983</v>
+      </c>
+      <c r="E149">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>5</v>
+      </c>
+      <c r="B150" s="1">
+        <v>43532</v>
+      </c>
+      <c r="D150">
+        <v>983</v>
+      </c>
+      <c r="E150">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <tableParts count="1">

</xml_diff>